<commit_message>
Scoring system added for sorting
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SortedByScoreTension" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,203 +436,1130 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SectionNamesC</t>
+          <t>SectionNames</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CompressionUtilization</t>
+          <t>Score</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>SectionNamesT</t>
+          <t>Mass</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>TensionUtilization</t>
+          <t>Deformation</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Utilization</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>W920x420</t>
+          <t>W690x419</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9967403509528058</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>W920x420</t>
-        </is>
+        <v>41643779.00026524</v>
+      </c>
+      <c r="C2" t="n">
+        <v>41643778.99999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9964678800935055</v>
+        <v>0.000265247</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9973732579454794</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>W920x449</t>
+          <t>W920x420</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9313326562374677</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>W920x449</t>
-        </is>
+        <v>41681616.00026549</v>
+      </c>
+      <c r="C3" t="n">
+        <v>41681616</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9310789825548756</v>
+        <v>0.000265488</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9964678800935055</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>W920x491</t>
+          <t>W360x421</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8533473323172154</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>W920x491</t>
-        </is>
+        <v>42010248.40026759</v>
+      </c>
+      <c r="C4" t="n">
+        <v>42010248.40000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8531168791537675</v>
+        <v>0.0002675812</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.988672838563638</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>W920x537</t>
+          <t>W460x421</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7790025077967097</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>W920x537</t>
-        </is>
+        <v>42068778.00026795</v>
+      </c>
+      <c r="C5" t="n">
+        <v>42068778</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7787931339989879</v>
+        <v>0.000267954</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.987297314278811</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>W920x588</t>
+          <t>W1000x438</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7101167693084333</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>W920x588</t>
-        </is>
+        <v>43059762.00027426</v>
+      </c>
+      <c r="C6" t="n">
+        <v>43059762</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7099276106693374</v>
+        <v>0.000274266</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.9645755017036912</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>W920x656</t>
+          <t>W840x433</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6359726163204991</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>W920x656</t>
-        </is>
+        <v>43114460.80027461</v>
+      </c>
+      <c r="C7" t="n">
+        <v>43114460.8</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6358044030408617</v>
+        <v>0.0002746144</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.963351756318185</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>W920x725</t>
+          <t>W1100x433</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5753635706720689</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>W920x725</t>
-        </is>
+        <v>43139502.30027477</v>
+      </c>
+      <c r="C8" t="n">
+        <v>43139502.3</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5752125589296351</v>
+        <v>0.0002747739</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.962792552532335</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W920x787</t>
+          <t>W760x434</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5298023318076484</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>W920x787</t>
-        </is>
+        <v>43175078.500275</v>
+      </c>
+      <c r="C9" t="n">
+        <v>43175078.5</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5296647279687614</v>
+        <v>0.0002750005</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.9619992129114842</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>W920x970</t>
+          <t>W1000x443</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4290486356603798</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>W920x970</t>
-        </is>
+        <v>43640599.20027797</v>
+      </c>
+      <c r="C10" t="n">
+        <v>43640599.2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4289396818671051</v>
+        <v>0.0002779656</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9517374256032564</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>W920x449</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>44608881.00028414</v>
+      </c>
+      <c r="C11" t="n">
+        <v>44608881.00000001</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0002841330000000001</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.9310789825548756</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>W310x454</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>45240554.80028816</v>
+      </c>
+      <c r="C12" t="n">
+        <v>45240554.8</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0002881564</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.9180787397061615</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>W610x455</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>45305804.00028857</v>
+      </c>
+      <c r="C13" t="n">
+        <v>45305804</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.000288572</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9167565271414571</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>W690x457</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>45550802.50029013</v>
+      </c>
+      <c r="C14" t="n">
+        <v>45550802.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0002901325</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.9118256815429658</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>W360x463</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>46127196.6002938</v>
+      </c>
+      <c r="C15" t="n">
+        <v>46127196.59999999</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0002938037999999999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.9004317321636568</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>W460x460</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>46290727.80029485</v>
+      </c>
+      <c r="C16" t="n">
+        <v>46290727.8</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0002948454</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.8972507780357588</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>W840x473</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>47113188.00030009</v>
+      </c>
+      <c r="C17" t="n">
+        <v>47113188</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.000300084</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.8815873707037514</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>W1000x483</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>47680272.00030369</v>
+      </c>
+      <c r="C18" t="n">
+        <v>47680272</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.000303696</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.8711022356246528</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>W1000x486</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>48010286.0003058</v>
+      </c>
+      <c r="C19" t="n">
+        <v>48010286</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.000305798</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.8651144368186336</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>W760x484</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>48264312.00030742</v>
+      </c>
+      <c r="C20" t="n">
+        <v>48264312</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.000307416</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.8605611436953984</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>W920x491</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>48685464.5003101</v>
+      </c>
+      <c r="C21" t="n">
+        <v>48685464.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0003100985</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.8531168791537675</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>W1000x494</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>48779900.0003107</v>
+      </c>
+      <c r="C22" t="n">
+        <v>48779900</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0003107</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.8514652866117302</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>W1100x499</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>49514032.00031538</v>
+      </c>
+      <c r="C23" t="n">
+        <v>49514032</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.000315376</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.8388408266648842</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>W610X498</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>49714285.50031665</v>
+      </c>
+      <c r="C24" t="n">
+        <v>49714285.5</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0003166515</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.8354619022814183</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>W690x500</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>49775751.00031704</v>
+      </c>
+      <c r="C25" t="n">
+        <v>49775751</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.000317043</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.8344302335969082</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>W310x500</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>49888068.80031776</v>
+      </c>
+      <c r="C26" t="n">
+        <v>49888068.8</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0003177583999999999</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.8325516006823567</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>W360x509</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>50790960.10032351</v>
+      </c>
+      <c r="C27" t="n">
+        <v>50790960.1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0003235093</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.8177516521171557</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>W840x527</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>52548999.0003347</v>
+      </c>
+      <c r="C28" t="n">
+        <v>52548998.99999999</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.000334707</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.7903935817006055</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>W760x531</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>52891887.0003369</v>
+      </c>
+      <c r="C29" t="n">
+        <v>52891887.00000001</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.000336891</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.7852696110916128</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>W920x537</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>53331738.20033968</v>
+      </c>
+      <c r="C30" t="n">
+        <v>53331738.19999999</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0003396925999999999</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.7787931339989879</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>W1000x539</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>53336762.20033972</v>
+      </c>
+      <c r="C31" t="n">
+        <v>53336762.2</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0003397246</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.7787197764020166</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>W360x79</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>54203622.00034525</v>
+      </c>
+      <c r="C32" t="n">
+        <v>54203622</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.000345246</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.7662659800555678</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>W690X548</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>54594081.00034774</v>
+      </c>
+      <c r="C33" t="n">
+        <v>54594081.00000001</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.000347733</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.7607856158324476</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>W1000x554</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>54799280.00034904</v>
+      </c>
+      <c r="C34" t="n">
+        <v>54799280</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.00034904</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.7579368111112323</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>W360x55Ι</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>54906982.00034972</v>
+      </c>
+      <c r="C35" t="n">
+        <v>54906982</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.000349726</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.7564500910720522</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>W610x551</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>55001401.80035032</v>
+      </c>
+      <c r="C36" t="n">
+        <v>55001401.8</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0003503274</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.7551515084183097</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>W840x576</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>57386797.00036552</v>
+      </c>
+      <c r="C37" t="n">
+        <v>57386797</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.000365521</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.7237621492342836</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>W1000x584</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>57848848.00036846</v>
+      </c>
+      <c r="C38" t="n">
+        <v>57848848</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.000368464</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.7179813076725665</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>W760x582</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>58018957.50036955</v>
+      </c>
+      <c r="C39" t="n">
+        <v>58018957.5</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0003695475</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.7158762122603036</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>W1000x591</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>58482814.00037249</v>
+      </c>
+      <c r="C40" t="n">
+        <v>58482813.99999999</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.000372502</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.7101982393390225</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>W920x588</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>58505108.00037264</v>
+      </c>
+      <c r="C41" t="n">
+        <v>58505108</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.000372644</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.7099276106693374</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>W360x592</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>59106261.00037646</v>
+      </c>
+      <c r="C42" t="n">
+        <v>59106260.99999999</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0003764729999999999</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.7027071384940342</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>W360x634</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>63273574.80040301</v>
+      </c>
+      <c r="C43" t="n">
+        <v>63273574.8</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0004030164</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.6564255562559352</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>W1000x642</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>63519374.00040457</v>
+      </c>
+      <c r="C44" t="n">
+        <v>63519373.99999999</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.000404582</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.6538854040720165</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>W920x656</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>65325737.50041609</v>
+      </c>
+      <c r="C45" t="n">
+        <v>65325737.5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0004160875</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.6358044030408617</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>W360x677</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>67626180.00043073</v>
+      </c>
+      <c r="C46" t="n">
+        <v>67626180</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.00043074</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.6141762189494</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>W920x725</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>72207031.80045992</v>
+      </c>
+      <c r="C47" t="n">
+        <v>72207031.8</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0004599174</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.5752125589296351</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>W360x744</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>74270985.20047307</v>
+      </c>
+      <c r="C48" t="n">
+        <v>74270985.2</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0004730636</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.5592276906324319</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>W1000x748</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>74371198.3004737</v>
+      </c>
+      <c r="C49" t="n">
+        <v>74371198.3</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.0004737019</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.5584741470326899</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>W920x787</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>78416381.80049948</v>
+      </c>
+      <c r="C50" t="n">
+        <v>78416381.80000001</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.0004994674</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.5296647279687614</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>W690x802</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>79985691.00050946</v>
+      </c>
+      <c r="C51" t="n">
+        <v>79985691</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.000509463</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.5192727726061844</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>W360x818</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>81748330.00052069</v>
+      </c>
+      <c r="C52" t="n">
+        <v>81748330</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.00052069</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.5080763305426733</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>W1000x883</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>87731600.00055879</v>
+      </c>
+      <c r="C53" t="n">
+        <v>87731600</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.0005588</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.473425670276064</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>W360x900</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>90059988.50057364</v>
+      </c>
+      <c r="C54" t="n">
+        <v>90059988.5</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.0005736305000000001</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.4611858409730036</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>W920x970</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>96830378.00061676</v>
+      </c>
+      <c r="C55" t="n">
+        <v>96830378</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.000616754</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.4289396818671051</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>W360x990</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>98947680.00063024</v>
+      </c>
+      <c r="C56" t="n">
+        <v>98947680</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.00063024</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.4197611458337531</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>W360x1086</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>108629870.0006919</v>
+      </c>
+      <c r="C57" t="n">
+        <v>108629870</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.00069191</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.3823477974740422</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>W920x1191</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0.3485510851213736</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>W920x1191</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+      <c r="B58" t="n">
+        <v>119192437.5007592</v>
+      </c>
+      <c r="C58" t="n">
+        <v>119192437.5</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0007591875</v>
+      </c>
+      <c r="E58" t="n">
         <v>0.3484649899402513</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>W610x217</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>143602405.0009147</v>
+      </c>
+      <c r="C59" t="n">
+        <v>143602405</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0009146649999999999</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.2892318658200156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>